<commit_message>
DN node 7. RES updated
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee18_2/ieee18_2_2020.xlsx
+++ b/data/IEEE9/ieee18_2/ieee18_2_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee18_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61693330-E8B8-4404-94DE-EC5254756F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD0A2AF-79D4-4C35-A675-7F53F210BA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26865" yWindow="3390" windowWidth="21600" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8700" yWindow="4965" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -8898,7 +8898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -13486,11 +13486,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.2663934426229492E-6</v>
+        <v>8.7213114754098344E-6</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4359818353600928E-6</v>
+        <v>5.1746365548139341E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13510,31 +13510,31 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6481596993183522E-3</v>
+        <v>8.2242303022929415E-3</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16628940577952522</v>
+        <v>0.17495031233054217</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41928900612391867</v>
+        <v>0.4447004610405198</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56737129056278046</v>
+        <v>0.54467643894026918</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.66396941715415791</v>
+        <v>0.61338127108526963</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65636898498201179</v>
+        <v>0.6629989747293048</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55414299240296594</v>
+        <v>0.55991531524049687</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13542,23 +13542,23 @@
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2502047927278952</v>
+        <v>0.24277296720132402</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1933967924761654E-2</v>
+        <v>5.6307354697373163E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6568140814081463E-4</v>
+        <v>3.6216524075484527E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8833503957839012E-5</v>
+        <v>5.8220654958278186E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5675916613330893E-5</v>
+        <v>1.6322346164396085E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13583,71 +13583,71 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4831693396692116</v>
+        <v>1.5137501507964117</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3343782849264372</v>
+        <v>1.4038771539330224</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.33698738982139</v>
+        <v>1.4052010321592161</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4084162835554688</v>
+        <v>1.2990247275511602</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1841616284124719</v>
+        <v>1.1604783958442224</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0765081848783828</v>
+        <v>1.0974112564294194</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.96441210835928715</v>
+        <v>0.93685747669187891</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.84115382100250269</v>
+        <v>0.83290721491424291</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83967814076405478</v>
+        <v>0.8235304842108998</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76679698285021258</v>
+        <v>0.7078125995540423</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7539420028679521</v>
+        <v>0.70319590652107067</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75850602690186608</v>
+        <v>0.68626735767311697</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.6696292920198782</v>
+        <v>0.66286535977725325</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69979810583149782</v>
+        <v>0.65314489877606463</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8058691296217384</v>
+        <v>0.88141936052377645</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.91571751422173753</v>
+        <v>0.95309373929201247</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94723275663302431</v>
+        <v>0.97652861508559219</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13655,7 +13655,7 @@
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0586218606005735</v>
+        <v>1.0483439784588204</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13663,11 +13663,11 @@
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1062904185486513</v>
+        <v>1.0509758976212185</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1919627790303129</v>
+        <v>1.0784425143607592</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13675,7 +13675,7 @@
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1793673547606227</v>
+        <v>1.191781747968629</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -13688,11 +13688,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5423497267759557E-6</v>
+        <v>4.4060792349726766E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7179909176800464E-6</v>
+        <v>2.5350492212977355E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13712,7 +13712,7 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0697222114439296E-3</v>
+        <v>4.4088657290642583E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13720,47 +13720,47 @@
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2223502305202599</v>
+        <v>0.21811498803415971</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28368564528139023</v>
+        <v>0.28935935818701802</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30036711728402377</v>
+        <v>0.30352887641332932</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34144447198559197</v>
+        <v>0.3314994873646524</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27707149620148297</v>
+        <v>0.27995765762024843</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23979191624774709</v>
+        <v>0.21923832342651159</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.1251023963639476</v>
+        <v>0.12014784601290016</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7880340675398362E-2</v>
+        <v>2.5966983962380827E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7580836929846858E-4</v>
+        <v>1.6877603452652984E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0029600978480329E-5</v>
+        <v>3.2174572476943211E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4035841638474901E-6</v>
+        <v>7.8379583066654464E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13789,11 +13789,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.4515027322404369E-6</v>
+        <v>4.5423497267759557E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6395873335161986E-6</v>
+        <v>2.6918563896254302E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13817,51 +13817,51 @@
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6609065510169392E-2</v>
+        <v>9.0073428130576172E-2</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20752688181890924</v>
+        <v>0.20329163933280905</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28652250173420413</v>
+        <v>0.27517507592294854</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30352887641332932</v>
+        <v>0.32249943118916241</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34807446173288503</v>
+        <v>0.3281844924910059</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28861614187654477</v>
+        <v>0.2828438190390139</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22380578849789726</v>
+        <v>0.23065698610497576</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12386375877618573</v>
+        <v>0.1189092084251383</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8427014021974801E-2</v>
+        <v>2.7060330655533704E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6877603452652984E-4</v>
+        <v>1.7756645299145325E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0029600978480329E-5</v>
+        <v>3.2174572476943211E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.9187620005485967E-6</v>
+        <v>7.8379583066654464E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13890,11 +13890,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5877732240437152E-6</v>
+        <v>4.6331967213114746E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6657218615708144E-6</v>
+        <v>2.5089146932431193E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13914,27 +13914,27 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3664727893617172E-3</v>
+        <v>4.1969010305515529E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4876884199966002E-2</v>
+        <v>8.6609065510169392E-2</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22023260927720981</v>
+        <v>0.20964450306195934</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28084878882857633</v>
+        <v>0.29219621463983192</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30985239467194031</v>
+        <v>0.33198470857707896</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.3314994873646524</v>
+        <v>0.32155450274371283</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13942,15 +13942,15 @@
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22837325356928292</v>
+        <v>0.21695459089081875</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12881830912723316</v>
+        <v>0.12138648360066201</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7060330655533704E-2</v>
+        <v>2.8427014021974801E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13958,7 +13958,7 @@
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9110327479139093E-5</v>
+        <v>3.0642449978041152E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14160,11 +14160,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.5389344262295074E-6</v>
+        <v>8.7213114754098344E-6</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1746365548139341E-6</v>
+        <v>5.2791746670323972E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14184,11 +14184,11 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3090161816980236E-3</v>
+        <v>8.6481596993183522E-3</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16802158708972861</v>
+        <v>0.16455722446932183</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14196,39 +14196,39 @@
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57304500346840825</v>
+        <v>0.55035015184589708</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64499886237832482</v>
+        <v>0.65132238063693582</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63647901574013255</v>
+        <v>0.68288894397118394</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5656876380780278</v>
+        <v>0.60032157510321316</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.45217904206718018</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25515934307894261</v>
+        <v>0.25268206790341891</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4667334657643847E-2</v>
+        <v>5.2480641271338092E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6568140814081463E-4</v>
+        <v>3.5513290598290651E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8220654958278186E-5</v>
+        <v>6.0672050956521478E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14257,99 +14257,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4525885285420115</v>
+        <v>1.5137501507964117</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4177769277343395</v>
+        <v>1.4316767015356566</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.391558303691651</v>
+        <v>1.3779155752240857</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4084162835554688</v>
+        <v>1.3537205055533144</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1249535469918484</v>
+        <v>1.2196864772648461</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0660566491028645</v>
+        <v>0.99289589867423644</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88174821335706244</v>
+        <v>0.87256333613459303</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86589363926728224</v>
+        <v>0.80816739664946347</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79123517110459007</v>
+        <v>0.7750875145514351</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7741700307622339</v>
+        <v>0.7078125995540423</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70319590652107067</v>
+        <v>0.7466925605326834</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70071509151886668</v>
+        <v>0.75128215997899117</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.67639322426250326</v>
+        <v>0.69668502099037843</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65314489877606463</v>
+        <v>0.63315066718087898</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82265806982219136</v>
+        <v>0.79747465952151197</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94374968302444384</v>
+        <v>0.97178185182714993</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.93746747048216839</v>
+        <v>0.94723275663302431</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1025606636392795</v>
+        <v>1.124179500181226</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.99695456775005464</v>
+        <v>1.0277882141753141</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.9990426077463459</v>
+        <v>1.0516237976277325</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0509758976212185</v>
+        <v>1.0620388018067051</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1465546731624914</v>
+        <v>1.1579066996294469</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0655926182456794</v>
+        <v>1.1315055637041751</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2786825004246751</v>
+        <v>1.3035112868406882</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -14362,11 +14362,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.4060792349726766E-6</v>
+        <v>4.5877732240437152E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.587318277406967E-6</v>
+        <v>2.6134528054615828E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14386,7 +14386,7 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1969010305515529E-3</v>
+        <v>4.0697222114439296E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14394,47 +14394,47 @@
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20329163933280905</v>
+        <v>0.20752688181890924</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26950136301732069</v>
+        <v>0.28935935818701802</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33198470857707896</v>
+        <v>0.30036711728402377</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32486949761735934</v>
+        <v>0.34144447198559197</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30016078755160658</v>
+        <v>0.29150230329531024</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22152205596220442</v>
+        <v>0.23294071864066859</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11767057083737643</v>
+        <v>0.12757967153947131</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7607004002110143E-2</v>
+        <v>2.6240320635669046E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.740502856054839E-4</v>
+        <v>1.7932453668443796E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0948874477821565E-5</v>
+        <v>2.9110327479139093E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.7571546127822977E-6</v>
+        <v>8.2419767760811911E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14463,11 +14463,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.4060792349726766E-6</v>
+        <v>4.5877732240437152E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4827801651885035E-6</v>
+        <v>2.6395873335161986E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14487,55 +14487,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3664727893617172E-3</v>
+        <v>4.4088657290642583E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.0939518785677867E-2</v>
+        <v>8.3144702889762612E-2</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21176212430500943</v>
+        <v>0.21387974554805952</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26950136301732069</v>
+        <v>0.29503307109264587</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30036711728402377</v>
+        <v>0.30985239467194031</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34807446173288503</v>
+        <v>0.34475946685923853</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2741853347827175</v>
+        <v>0.27995765762024843</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22152205596220442</v>
+        <v>0.23294071864066859</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12014784601290016</v>
+        <v>0.12881830912723316</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7060330655533704E-2</v>
+        <v>2.7607004002110143E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7053411821951452E-4</v>
+        <v>1.6701795083354514E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2174572476943211E-5</v>
+        <v>2.9110327479139093E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.7571546127822977E-6</v>
+        <v>7.6763509188991491E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14564,11 +14564,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.7240437158469943E-6</v>
+        <v>4.6786202185792349E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6395873335161986E-6</v>
+        <v>2.5611837493523513E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14588,23 +14588,23 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3664727893617172E-3</v>
+        <v>4.1969010305515529E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6609065510169392E-2</v>
+        <v>8.4876884199966002E-2</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20964450306195934</v>
+        <v>0.20540926057585915</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27517507592294854</v>
+        <v>0.29786992754545977</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31933767205985686</v>
+        <v>0.31301415380124586</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14612,23 +14612,23 @@
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27707149620148297</v>
+        <v>0.30304694897037204</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23294071864066859</v>
+        <v>0.21923832342651159</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12634103395170945</v>
+        <v>0.12757967153947131</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7060330655533704E-2</v>
+        <v>2.8153677348686582E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8284070407040731E-4</v>
+        <v>1.8108262037742264E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14636,7 +14636,7 @@
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.7571546127822977E-6</v>
+        <v>8.3227804699643415E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14834,11 +14834,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.2663934426229492E-6</v>
+        <v>8.9938524590163926E-6</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2791746670323972E-6</v>
+        <v>5.0178293864862386E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14858,15 +14858,15 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.5633738199132701E-3</v>
+        <v>8.1394444228878593E-3</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17841467495094895</v>
+        <v>0.169753768399932</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41505376363781848</v>
+        <v>0.42775949109611905</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14874,39 +14874,39 @@
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63867534411971372</v>
+        <v>0.61970478934388062</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62984902599283954</v>
+        <v>0.66962896447659781</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5656876380780278</v>
+        <v>0.57723228375308955</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.47958383249549419</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26011389342999003</v>
+        <v>0.24772751755237146</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1933967924761654E-2</v>
+        <v>5.2480641271338092E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5864907336887592E-4</v>
+        <v>3.481005712109678E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2510597955203957E-5</v>
+        <v>6.4349144953886422E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6483953552162382E-5</v>
+        <v>1.5675916613330893E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14931,75 +14931,75 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4984597452328119</v>
+        <v>1.5443309619236123</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4177769277343395</v>
+        <v>1.32047851112512</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3779155752240857</v>
+        <v>1.391558303691651</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3810683945543913</v>
+        <v>1.3126986720516987</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2078448609807213</v>
+        <v>1.172320012128347</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0556051133273463</v>
+        <v>1.0765081848783828</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.9276725994694095</v>
+        <v>0.91848772224694009</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83290721491424291</v>
+        <v>0.85764703317902247</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8235304842108998</v>
+        <v>0.83160431248747735</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.73730479120212744</v>
+        <v>0.72993174329010624</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71044534885633948</v>
+        <v>0.69594646418580197</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69349122459599177</v>
+        <v>0.75850602690186608</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70344895323300349</v>
+        <v>0.68992108874775337</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65314489877606463</v>
+        <v>0.65980964264112651</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8058691296217384</v>
+        <v>0.8646304203233236</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.95309373929201247</v>
+        <v>0.97178185182714993</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94723275663302431</v>
+        <v>1.015589759689016</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.026894735742466</v>
+        <v>1.0809418270973328</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -15007,11 +15007,11 @@
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0095588457226232</v>
+        <v>1.1042049875091191</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0841646101776783</v>
+        <v>1.1062904185486513</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -15019,11 +15019,11 @@
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0655926182456794</v>
+        <v>1.087563600065178</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2290249275926488</v>
+        <v>1.2662681072166684</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -15036,11 +15036,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.6331967213114746E-6</v>
+        <v>4.3152322404371578E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7179909176800464E-6</v>
+        <v>2.587318277406967E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15060,55 +15060,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.281686909956635E-3</v>
+        <v>4.0697222114439296E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4010793544864307E-2</v>
+        <v>8.7475156165271087E-2</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21811498803415971</v>
+        <v>0.21176212430500943</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28652250173420413</v>
+        <v>0.28084878882857633</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30669063554263482</v>
+        <v>0.31617591293055136</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31492451299641977</v>
+        <v>0.31823950787006627</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29727462613284111</v>
+        <v>0.27707149620148297</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22380578849789726</v>
+        <v>0.23294071864066859</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12634103395170945</v>
+        <v>0.1251023963639476</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8427014021974801E-2</v>
+        <v>2.5966983962380827E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8459878776339202E-4</v>
+        <v>1.7229220191249919E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9723176478699916E-5</v>
+        <v>2.9110327479139093E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.2419767760811911E-6</v>
+        <v>7.6763509188991491E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15137,11 +15137,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.6786202185792349E-6</v>
+        <v>4.3152322404371578E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.587318277406967E-6</v>
+        <v>2.6395873335161986E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15161,35 +15161,35 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.281686909956635E-3</v>
+        <v>4.0697222114439296E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.0939518785677867E-2</v>
+        <v>8.2278612234660917E-2</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2223502305202599</v>
+        <v>0.21176212430500943</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29786992754545977</v>
+        <v>0.28084878882857633</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32249943118916241</v>
+        <v>0.30352887641332932</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31492451299641977</v>
+        <v>0.34144447198559197</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30304694897037204</v>
+        <v>0.2741853347827175</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22380578849789726</v>
+        <v>0.23294071864066859</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15197,19 +15197,19 @@
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8427014021974801E-2</v>
+        <v>2.7607004002110143E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8108262037742264E-4</v>
+        <v>1.6877603452652984E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1255298977601978E-5</v>
+        <v>3.0029600978480329E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.6763509188991491E-6</v>
+        <v>7.9187620005485967E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15238,11 +15238,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.4969262295081963E-6</v>
+        <v>4.5877732240437152E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6918563896254302E-6</v>
+        <v>2.6657218615708144E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15262,55 +15262,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0697222114439296E-3</v>
+        <v>4.1545080908490118E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.0073428130576172E-2</v>
+        <v>8.4876884199966002E-2</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20752688181890924</v>
+        <v>0.22023260927720981</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28935935818701802</v>
+        <v>0.28652250173420413</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30036711728402377</v>
+        <v>0.32249943118916241</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.3314994873646524</v>
+        <v>0.3348144822382989</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30304694897037204</v>
+        <v>0.28861614187654477</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21695459089081875</v>
+        <v>0.23750818371205426</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12138648360066201</v>
+        <v>0.12262512118842388</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7880340675398362E-2</v>
+        <v>2.8427014021974801E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8108262037742264E-4</v>
+        <v>1.7053411821951452E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0642449978041152E-5</v>
+        <v>3.1255298977601978E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.2419767760811911E-6</v>
+        <v>8.3227804699643415E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -17000,7 +17000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303073B7-556E-4714-A27A-3E87EB1A31BB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -26461,11 +26461,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.130681693989071E-5</v>
+        <v>1.1076065573770491E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.5200420590655566E-6</v>
+        <v>6.3224650269726606E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26485,55 +26485,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0465189323904138E-2</v>
+        <v>1.0888025256183095E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21421278566858662</v>
+        <v>0.22732785417890827</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5231666262507465</v>
+        <v>0.53934703737190359</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71217844620645809</v>
+        <v>0.72671270021067158</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.78349321434327002</v>
+        <v>0.83146218665000093</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86743119648043332</v>
+        <v>0.85900953437868155</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.74468363777208013</v>
+        <v>0.77417605906998432</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55112869150396182</v>
+        <v>0.59705608246262531</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.3042749416436209</v>
+        <v>0.31979917336013219</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.8046838570399337E-2</v>
+        <v>7.2907327039713574E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5658671045591245E-4</v>
+        <v>4.3902568313068505E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.4438097284447284E-5</v>
+        <v>7.2934297339306934E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9358948980524821E-5</v>
+        <v>1.8967859102130381E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26558,15 +26558,15 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1909315862190484</v>
+        <v>1.1682471750529713</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0374297050554147</v>
+        <v>0.95762742005115198</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.086234686340535</v>
+        <v>1.0131227362983837</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26574,19 +26574,19 @@
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.91476485794863471</v>
+        <v>0.92364607016172828</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7929433407780353</v>
+        <v>0.83259050781693711</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69914623893691652</v>
+        <v>0.71341452952746587</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65932144309674001</v>
+        <v>0.67212380121512338</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26594,11 +26594,11 @@
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54470347735582203</v>
+        <v>0.53380940780870556</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56577357671134909</v>
+        <v>0.52694597830958978</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26606,43 +26606,43 @@
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47959529303899939</v>
+        <v>0.50457421455144735</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.49626733590700584</v>
+        <v>0.48613943109257712</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62183133733283102</v>
+        <v>0.65292290419947263</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.73235334268891561</v>
+        <v>0.68352978650965457</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71616650131849258</v>
+        <v>0.66701781985545883</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80891838411314465</v>
+        <v>0.76926552214681387</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.78461792075552139</v>
+        <v>0.72426269608201965</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7951588989085745</v>
+        <v>0.74792173659717409</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86438487446773749</v>
+        <v>0.87302872321241498</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80615472782578956</v>
+        <v>0.8733342884779387</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26650,7 +26650,7 @@
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8850361759249149</v>
+        <v>0.94093319756227811</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -26663,11 +26663,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6534084699453549E-6</v>
+        <v>5.7687841530054644E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3258800402304106E-6</v>
+        <v>3.2270915241839626E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26687,23 +26687,23 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3911581365566775E-3</v>
+        <v>5.3383036450218085E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11147808233773386</v>
+        <v>0.10929223758601359</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28315719462024941</v>
+        <v>0.2696735186859518</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.38152416761060259</v>
+        <v>0.37789060410954922</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41173367896610624</v>
+        <v>0.38774919281274078</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26711,31 +26711,31 @@
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35022250291261198</v>
+        <v>0.38708802953499216</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27556434575198091</v>
+        <v>0.28991665542656325</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16145200985171723</v>
+        <v>0.15679474033676385</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5759308024240467E-2</v>
+        <v>3.4370597033007828E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1073232790272883E-4</v>
+        <v>2.2170796998099597E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6467148669653467E-5</v>
+        <v>3.6091198683368379E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.8750194294596327E-6</v>
+        <v>9.972791899058242E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26764,11 +26764,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.7110963114754101E-6</v>
+        <v>5.5957206284153006E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2929505348815944E-6</v>
+        <v>3.1283030081375146E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26788,31 +26788,31 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1797401704171998E-3</v>
+        <v>5.3911581365566775E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10929223758601359</v>
+        <v>0.1038276257067129</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25618984275165418</v>
+        <v>0.28046045943338987</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.38152416761060259</v>
+        <v>0.35608922310322905</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37975436409495233</v>
+        <v>0.39574402153052929</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44213726034196849</v>
+        <v>0.40423978088408541</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36128216089932602</v>
+        <v>0.38708802953499216</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26820,23 +26820,23 @@
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14748020130685707</v>
+        <v>0.15524231716511272</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2981886041775189E-2</v>
+        <v>3.3676241537391509E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0853719948707539E-4</v>
+        <v>2.1731771314968909E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7594998628508729E-5</v>
+        <v>3.6467148669653467E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.28838461186797E-6</v>
+        <v>9.7772469598610216E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26865,11 +26865,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.7110963114754101E-6</v>
+        <v>5.4803449453551911E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2600210295327783E-6</v>
+        <v>3.1941620188351465E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26889,55 +26889,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.12688567888233E-3</v>
+        <v>5.4440126280915473E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10601347045843318</v>
+        <v>0.10929223758601359</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25618984275165418</v>
+        <v>0.27237025387281133</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37062347710744253</v>
+        <v>0.37425704060849585</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37975436409495233</v>
+        <v>0.40373885024831774</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.40845061193496135</v>
+        <v>0.41266144298583723</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37971492421051611</v>
+        <v>0.36496871356156407</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28417573155673032</v>
+        <v>0.27269388381706444</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16300443302336837</v>
+        <v>0.15679474033676385</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4717774780815988E-2</v>
+        <v>3.3676241537391509E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1073232790272883E-4</v>
+        <v>2.1292745631838224E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9098798573649079E-5</v>
+        <v>3.9474748559934167E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0266109307854073E-5</v>
+        <v>9.28838461186797E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27216,11 +27216,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1537568306010929E-5</v>
+        <v>1.2114446721311475E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.3224650269726606E-6</v>
+        <v>6.5200420590655566E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27240,27 +27240,27 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0042353391625182E-2</v>
+        <v>1.0570898306973877E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22951369893062853</v>
+        <v>0.21421278566858662</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52856009662446546</v>
+        <v>0.56631438924049882</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71944557320856484</v>
+        <v>0.71217844620645809</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81547252921442404</v>
+        <v>0.79148804306105858</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.84216621017517801</v>
+        <v>0.82532288597167447</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27272,23 +27272,23 @@
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31048463433022544</v>
+        <v>0.31979917336013219</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1518616048480935E-2</v>
+        <v>7.2907327039713574E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3902568313068505E-4</v>
+        <v>4.2146465580545766E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.5189997257017459E-5</v>
+        <v>7.7445697174727984E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9945583798116484E-5</v>
+        <v>1.857676922373594E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27313,39 +27313,39 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1569049694699327</v>
+        <v>1.1795893806360098</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0474049906809475</v>
+        <v>0.96760270567668472</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0653455577570632</v>
+        <v>1.0444564291735914</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.036407751893754</v>
+        <v>1.0464699630771885</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.90588364573554114</v>
+        <v>0.8614775846700734</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7691550405546943</v>
+        <v>0.80087277418581571</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70628038423219119</v>
+        <v>0.6777438030510925</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65292026403754855</v>
+        <v>0.64011790591916518</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58660819677056475</v>
+        <v>0.6221602086960536</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27353,7 +27353,7 @@
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52694597830958978</v>
+        <v>0.57132037648302891</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27361,15 +27361,15 @@
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47459950873650986</v>
+        <v>0.47959529303899939</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52665105035029203</v>
+        <v>0.50133128831422025</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65292290419947263</v>
+        <v>0.59073977046618942</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27377,7 +27377,7 @@
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.66701781985545883</v>
+        <v>0.69510278069147802</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27385,27 +27385,27 @@
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72426269608201965</v>
+        <v>0.7695291145871459</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81090461967904137</v>
+        <v>0.80303175929380799</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.84709717697838283</v>
+        <v>0.90760411819112441</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.85653939831490145</v>
+        <v>0.88173173355945744</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83949929680030699</v>
+        <v>0.83126891153755889</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94093319756227811</v>
+        <v>0.97819787865385355</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27418,11 +27418,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8264719945355187E-6</v>
+        <v>5.7110963114754101E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4575980616256742E-6</v>
+        <v>3.4246685562768585E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27442,55 +27442,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1797401704171998E-3</v>
+        <v>5.3911581365566775E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10492054808257303</v>
+        <v>0.10710639283429331</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27506698905967086</v>
+        <v>0.27776372424653034</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36698991360638916</v>
+        <v>0.37425704060849585</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.39974143588942351</v>
+        <v>0.38774919281274078</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41266144298583723</v>
+        <v>0.44213726034196849</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36128216089932602</v>
+        <v>0.35390905557484997</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28130526962181385</v>
+        <v>0.27556434575198091</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15524231716511272</v>
+        <v>0.15058504765015934</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5759308024240467E-2</v>
+        <v>3.6106485772048627E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1073232790272883E-4</v>
+        <v>2.2829335522795623E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8722848587363992E-5</v>
+        <v>3.7219048642223642E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.28838461186797E-6</v>
+        <v>9.8750194294596327E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27519,11 +27519,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.7110963114754101E-6</v>
+        <v>6.0572233606557376E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2270915241839626E-6</v>
+        <v>3.2600210295327783E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27543,55 +27543,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1797401704171998E-3</v>
+        <v>5.3383036450218085E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11475684946531427</v>
+        <v>0.10819931521015345</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26158331312537325</v>
+        <v>0.28046045943338987</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35245565960217573</v>
+        <v>0.34518853260006899</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.38774919281274078</v>
+        <v>0.39974143588942351</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44213726034196849</v>
+        <v>0.421083105087589</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36128216089932602</v>
+        <v>0.36865526622380207</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27843480768689738</v>
+        <v>0.29278711736147972</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15524231716511272</v>
+        <v>0.15368989399346158</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6453663519856787E-2</v>
+        <v>3.6106485772048627E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1512258473403568E-4</v>
+        <v>2.3048848364360966E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9098798573649079E-5</v>
+        <v>3.5715248697083292E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.28838461186797E-6</v>
+        <v>9.4839295510651903E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27620,11 +27620,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4803449453551911E-6</v>
+        <v>5.7687841530054644E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3258800402304106E-6</v>
+        <v>3.1283030081375146E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27644,11 +27644,11 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4968671196264163E-3</v>
+        <v>5.0211766958125912E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10929223758601359</v>
+        <v>0.10710639283429331</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27656,43 +27656,43 @@
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36698991360638916</v>
+        <v>0.37062347710744253</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.38774919281274078</v>
+        <v>0.37975436409495233</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4379264292910926</v>
+        <v>0.43371559824021666</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37602837154827812</v>
+        <v>0.36496871356156407</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28130526962181385</v>
+        <v>0.27556434575198091</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15368989399346158</v>
+        <v>0.15679474033676385</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5412130276432308E-2</v>
+        <v>3.4370597033007828E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1292745631838224E-4</v>
+        <v>2.2609822681230282E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7219048642223642E-5</v>
+        <v>3.7594998628508729E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.4839295510651903E-6</v>
+        <v>9.28838461186797E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27890,11 +27890,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1999071038251367E-5</v>
+        <v>1.1076065573770491E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.849337112553717E-6</v>
+        <v>6.2566060162750292E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27914,27 +27914,27 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1099443222322572E-2</v>
+        <v>1.0993734239252833E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22514200942718798</v>
+        <v>0.22732785417890827</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5231666262507465</v>
+        <v>0.56092091886677975</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7485140812169917</v>
+        <v>0.69764419220224472</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75950872818990467</v>
+        <v>0.79148804306105858</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8758528585821852</v>
+        <v>0.82532288597167447</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27942,27 +27942,27 @@
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58557423472295944</v>
+        <v>0.55112869150396182</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32290401970343446</v>
+        <v>0.32600886604673673</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.0824260552864615E-2</v>
+        <v>6.8046838570399337E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3024516946807136E-4</v>
+        <v>4.2146465580545766E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2182397366736759E-5</v>
+        <v>7.8197597147298159E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.857676922373594E-5</v>
+        <v>1.9163404041327603E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27987,43 +27987,43 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1569049694699327</v>
+        <v>1.122878352720817</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0474049906809475</v>
+        <v>1.0374297050554147</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.99223360771491176</v>
+        <v>1.0549009934653273</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0062211183434506</v>
+        <v>1.0565321742606231</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8614775846700734</v>
+        <v>0.88812122130935411</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80880220759359611</v>
+        <v>0.81673164100137641</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69914623893691652</v>
+        <v>0.74195111070856457</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65932144309674001</v>
+        <v>0.67212380121512338</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.6221602086960536</v>
+        <v>0.58660819677056475</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5555975469029385</v>
+        <v>0.52836237303514733</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28039,11 +28039,11 @@
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.50133128831422025</v>
+        <v>0.51652314553586332</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59073977046618942</v>
+        <v>0.64048627745281594</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28055,15 +28055,15 @@
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75340437736028165</v>
+        <v>0.80098781171987854</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75444030841877052</v>
+        <v>0.79216232383970908</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82665034044950825</v>
+        <v>0.74792173659717409</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28071,15 +28071,15 @@
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82294961798882682</v>
+        <v>0.80615472782578956</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.78188659996107024</v>
+        <v>0.83126891153755889</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8850361759249149</v>
+        <v>0.94093319756227811</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -28092,11 +28092,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6534084699453549E-6</v>
+        <v>5.5380327868852455E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4246685562768585E-6</v>
+        <v>3.3588095455792263E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28116,23 +28116,23 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3911581365566775E-3</v>
+        <v>5.4968671196264163E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10710639283429331</v>
+        <v>0.10601347045843318</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26428004831223273</v>
+        <v>0.27506698905967086</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34518853260006899</v>
+        <v>0.35608922310322905</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41573109332500047</v>
+        <v>0.40773626460721202</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28140,31 +28140,31 @@
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37971492421051611</v>
+        <v>0.38340147687275417</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29278711736147972</v>
+        <v>0.29565757929639619</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.1598995866800661</v>
+        <v>0.16300443302336837</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2981886041775189E-2</v>
+        <v>3.6106485772048627E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2390309839664938E-4</v>
+        <v>2.1731771314968909E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9474748559934167E-5</v>
+        <v>3.7594998628508729E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.4839295510651903E-6</v>
+        <v>9.6794744902624106E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28193,11 +28193,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.9995355191256833E-6</v>
+        <v>5.5957206284153006E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4246685562768585E-6</v>
+        <v>3.2600210295327783E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28217,27 +28217,27 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.074031187347461E-3</v>
+        <v>5.1797401704171998E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11038515996187372</v>
+        <v>0.10601347045843318</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25618984275165418</v>
+        <v>0.27237025387281133</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37062347710744253</v>
+        <v>0.37425704060849585</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41573109332500047</v>
+        <v>0.37975436409495233</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.40423978088408541</v>
+        <v>0.421083105087589</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28245,27 +28245,27 @@
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27843480768689738</v>
+        <v>0.27269388381706444</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15213747082181045</v>
+        <v>0.16300443302336837</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4717774780815988E-2</v>
+        <v>3.2981886041775189E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1073232790272883E-4</v>
+        <v>2.2609822681230282E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6091198683368379E-5</v>
+        <v>3.9474748559934167E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.972791899058242E-6</v>
+        <v>9.28838461186797E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28294,11 +28294,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.7687841530054644E-6</v>
+        <v>5.9995355191256833E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3588095455792263E-6</v>
+        <v>3.2270915241839626E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28318,35 +28318,35 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3911581365566775E-3</v>
+        <v>5.4440126280915473E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10492054808257303</v>
+        <v>0.10710639283429331</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25618984275165418</v>
+        <v>0.27237025387281133</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.38152416761060259</v>
+        <v>0.36698991360638916</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.40373885024831774</v>
+        <v>0.39574402153052929</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41266144298583723</v>
+        <v>0.40002894983320952</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36865526622380207</v>
+        <v>0.36496871356156407</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28991665542656325</v>
+        <v>0.28130526962181385</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28354,19 +28354,19 @@
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4370597033007828E-2</v>
+        <v>3.2981886041775189E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3048848364360966E-4</v>
+        <v>2.1951284156534253E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5715248697083292E-5</v>
+        <v>3.7594998628508729E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.28838461186797E-6</v>
+        <v>1.0070564368656853E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>

</xml_diff>

<commit_message>
ADN node 7. Flex growth modified
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee18_2/ieee18_2_2020.xlsx
+++ b/data/IEEE9/ieee18_2/ieee18_2_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee18_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C5F4CE-0671-4C5E-99DA-3AC589E76108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8E6D37-543F-42F2-AA17-21A728061662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="4965" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23760" yWindow="5520" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -249,12 +249,12 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>2.5000000000000001E-2</v>
+            <v>0.02</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.15</v>
+            <v>0.09</v>
           </cell>
         </row>
       </sheetData>
@@ -8899,7 +8899,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13486,11 +13486,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.9030054644808738E-6</v>
+        <v>9.5389344262295074E-6</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4359818353600928E-6</v>
+        <v>5.4882508914693243E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13510,55 +13510,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6481596993183522E-3</v>
+        <v>8.8177314581285166E-3</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16628940577952522</v>
+        <v>0.18187903757135573</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42775949109611905</v>
+        <v>0.40658327866561811</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57304500346840825</v>
+        <v>0.56169757765715267</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63867534411971372</v>
+        <v>0.60705775282665864</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64310900548742567</v>
+        <v>0.68951893371847706</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55991531524049687</v>
+        <v>0.5656876380780278</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45674650713856585</v>
+        <v>0.47044890235272285</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24029569202580031</v>
+        <v>0.24772751755237146</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3027314617914531E-2</v>
+        <v>5.2480641271338092E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4106823643902904E-4</v>
+        <v>3.3755206905305968E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8833503957839012E-5</v>
+        <v>6.0059201956960658E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5514309225564595E-5</v>
+        <v>1.680716832769498E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13583,23 +13583,23 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5749117730508124</v>
+        <v>1.4525885285420115</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4177769277343395</v>
+        <v>1.4316767015356566</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3642728467565204</v>
+        <v>1.2960592044186945</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2990247275511602</v>
+        <v>1.4084162835554688</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2078448609807213</v>
+        <v>1.1249535469918484</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13607,35 +13607,35 @@
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.95522723113681773</v>
+        <v>0.94604235391434832</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.85764703317902247</v>
+        <v>0.78342757838468391</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81545665593432237</v>
+        <v>0.79123517110459007</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7151856474660635</v>
+        <v>0.75942393493819138</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69594646418580197</v>
+        <v>0.7466925605326834</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.74405829305611626</v>
+        <v>0.71516282536461651</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69668502099037843</v>
+        <v>0.70344895323300349</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69313336196643593</v>
+        <v>0.6664743865061884</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13643,39 +13643,39 @@
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.95309373929201247</v>
+        <v>0.92506157048930615</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0253550458398717</v>
+        <v>0.97652861508559219</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0485135722844128</v>
+        <v>1.026894735742466</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0277882141753141</v>
+        <v>1.0688997427423266</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0516237976277325</v>
+        <v>1.0936887495328418</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1394791311051107</v>
+        <v>1.0620388018067051</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1919627790303129</v>
+        <v>1.0897945408277145</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0546071273359301</v>
+        <v>1.1424910546139244</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3035112868406882</v>
+        <v>1.2290249275926488</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -13688,11 +13688,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.7240437158469943E-6</v>
+        <v>4.4515027322404369E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6657218615708144E-6</v>
+        <v>2.7441254457346622E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13712,55 +13712,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0697222114439296E-3</v>
+        <v>4.239293970254094E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.7475156165271087E-2</v>
+        <v>9.0073428130576172E-2</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2223502305202599</v>
+        <v>0.21387974554805952</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29503307109264587</v>
+        <v>0.28652250173420413</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31301415380124586</v>
+        <v>0.30352887641332932</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32155450274371283</v>
+        <v>0.31492451299641977</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30016078755160658</v>
+        <v>0.29150230329531024</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23979191624774709</v>
+        <v>0.22152205596220442</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.1251023963639476</v>
+        <v>0.11767057083737643</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6240320635669046E-2</v>
+        <v>2.870035069526302E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7580836929846858E-4</v>
+        <v>1.740502856054839E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0029600978480329E-5</v>
+        <v>3.0948874477821565E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.9187620005485967E-6</v>
+        <v>7.6763509188991491E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13789,11 +13789,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.7694672131147537E-6</v>
+        <v>4.6331967213114746E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7441254457346622E-6</v>
+        <v>2.4827801651885035E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13813,55 +13813,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.281686909956635E-3</v>
+        <v>4.0273292717413894E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.5742974855067697E-2</v>
+        <v>9.0073428130576172E-2</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20752688181890924</v>
+        <v>0.20329163933280905</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28084878882857633</v>
+        <v>0.27233821947013459</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31933767205985686</v>
+        <v>0.31617591293055136</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34144447198559197</v>
+        <v>0.31492451299641977</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2741853347827175</v>
+        <v>0.28861614187654477</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23979191624774709</v>
+        <v>0.22152205596220442</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12014784601290016</v>
+        <v>0.13005694671499501</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8153677348686582E-2</v>
+        <v>2.870035069526302E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8459878776339202E-4</v>
+        <v>1.7053411821951452E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0948874477821565E-5</v>
+        <v>3.1868147977162798E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.9995656944317453E-6</v>
+        <v>8.4843878577306387E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13890,11 +13890,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5877732240437152E-6</v>
+        <v>4.4060792349726766E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6657218615708144E-6</v>
+        <v>2.5350492212977355E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13918,51 +13918,51 @@
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.8341246820372782E-2</v>
+        <v>8.5742974855067697E-2</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20329163933280905</v>
+        <v>0.22023260927720981</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28084878882857633</v>
+        <v>0.29219621463983192</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30985239467194031</v>
+        <v>0.31301415380124586</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34144447198559197</v>
+        <v>0.32486949761735934</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30304694897037204</v>
+        <v>0.28861614187654477</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23750818371205426</v>
+        <v>0.21923832342651159</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12014784601290016</v>
+        <v>0.12262512118842388</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6786993982245485E-2</v>
+        <v>2.6513657308957266E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8459878776339202E-4</v>
+        <v>1.7756645299145325E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0336025478260739E-5</v>
+        <v>3.1255298977601978E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.8379583066654464E-6</v>
+        <v>7.7571546127822977E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14160,11 +14160,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.7213114754098344E-6</v>
+        <v>8.9030054644808738E-6</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.965560330377007E-6</v>
+        <v>5.4882508914693243E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14184,7 +14184,7 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.8177314581285166E-3</v>
+        <v>8.2242303022929415E-3</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14192,39 +14192,39 @@
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4447004610405198</v>
+        <v>0.4108185211517183</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59006614218529174</v>
+        <v>0.53900272603464139</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60705775282665864</v>
+        <v>0.65132238063693582</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.68951893371847706</v>
+        <v>0.67625895422389093</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54837066956543501</v>
+        <v>0.60032157510321316</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47501636742410852</v>
+        <v>0.46131397220995152</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2378184168502766</v>
+        <v>0.23534114167475287</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.357398796449097E-2</v>
+        <v>5.1933967924761654E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.481005712109678E-4</v>
+        <v>3.3403590166709027E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14232,7 +14232,7 @@
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6483953552162382E-5</v>
+        <v>1.5675916613330893E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14257,31 +14257,31 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5902021786144127</v>
+        <v>1.4678789341056113</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4177769277343395</v>
+        <v>1.4594762491382907</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4052010321592161</v>
+        <v>1.3779155752240857</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3537205055533144</v>
+        <v>1.3126986720516987</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.172320012128347</v>
+        <v>1.2196864772648461</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0451535775518279</v>
+        <v>1.0033474344497548</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.91848772224694009</v>
+        <v>0.87256333613459303</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14289,23 +14289,23 @@
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7750875145514351</v>
+        <v>0.76701368627485766</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.73730479120212744</v>
+        <v>0.75942393493819138</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70319590652107067</v>
+        <v>0.7466925605326834</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.74405829305611626</v>
+        <v>0.73683442613324135</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69668502099037843</v>
+        <v>0.64933749529200302</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14313,11 +14313,11 @@
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88141936052377645</v>
+        <v>0.84784148012287064</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.92506157048930615</v>
+        <v>0.934405626756875</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14329,27 +14329,27 @@
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0791776248840799</v>
+        <v>1.0175103320335608</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0516237976277325</v>
+        <v>1.0831725115565645</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1505420352905973</v>
+        <v>1.0731017059921917</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1692587260964022</v>
+        <v>1.1352026466955361</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1205200727944258</v>
+        <v>1.1095345818846765</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2041961411766358</v>
+        <v>1.2414393208006553</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -14362,11 +14362,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5423497267759557E-6</v>
+        <v>4.3152322404371578E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.587318277406967E-6</v>
+        <v>2.6657218615708144E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14390,27 +14390,27 @@
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4010793544864307E-2</v>
+        <v>8.2278612234660917E-2</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22023260927720981</v>
+        <v>0.20329163933280905</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28935935818701802</v>
+        <v>0.28368564528139023</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33198470857707896</v>
+        <v>0.30352887641332932</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34144447198559197</v>
+        <v>0.3314994873646524</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28572998045777931</v>
+        <v>0.2828438190390139</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14418,19 +14418,19 @@
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12386375877618573</v>
+        <v>0.12138648360066201</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7333667328821924E-2</v>
+        <v>2.6513657308957266E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7932453668443796E-4</v>
+        <v>1.6877603452652984E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9110327479139093E-5</v>
+        <v>3.0029600978480329E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14463,11 +14463,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.6786202185792349E-6</v>
+        <v>4.7694672131147537E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.587318277406967E-6</v>
+        <v>2.5350492212977355E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14487,11 +14487,11 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1545080908490118E-3</v>
+        <v>4.1969010305515529E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.5742974855067697E-2</v>
+        <v>8.6609065510169392E-2</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14499,7 +14499,7 @@
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28368564528139023</v>
+        <v>0.28652250173420413</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14507,35 +14507,35 @@
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34144447198559197</v>
+        <v>0.34475946685923853</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29438846471407565</v>
+        <v>0.30016078755160658</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21695459089081875</v>
+        <v>0.22608952103359009</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12014784601290016</v>
+        <v>0.13005694671499501</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6513657308957266E-2</v>
+        <v>2.7607004002110143E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7756645299145325E-4</v>
+        <v>1.6877603452652984E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9416751978919506E-5</v>
+        <v>2.9723176478699916E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.9995656944317453E-6</v>
+        <v>8.2419767760811911E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14564,11 +14564,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.6786202185792349E-6</v>
+        <v>4.6331967213114746E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5611837493523513E-6</v>
+        <v>2.6918563896254302E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14588,35 +14588,35 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1969010305515529E-3</v>
+        <v>4.239293970254094E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.8341246820372782E-2</v>
+        <v>8.5742974855067697E-2</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21387974554805952</v>
+        <v>0.20964450306195934</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28935935818701802</v>
+        <v>0.27233821947013459</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.3288229494477734</v>
+        <v>0.30669063554263482</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34144447198559197</v>
+        <v>0.3314994873646524</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2741853347827175</v>
+        <v>0.2828438190390139</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23522445117636143</v>
+        <v>0.22152205596220442</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14624,19 +14624,19 @@
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8427014021974801E-2</v>
+        <v>2.5966983962380827E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6877603452652984E-4</v>
+        <v>1.740502856054839E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1868147977162798E-5</v>
+        <v>3.1255298977601978E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.9187620005485967E-6</v>
+        <v>7.8379583066654464E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14834,11 +14834,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.2663934426229492E-6</v>
+        <v>8.7213114754098344E-6</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.0178293864862386E-6</v>
+        <v>5.070098442595471E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14858,7 +14858,7 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.0546585434827789E-3</v>
+        <v>8.5633738199132701E-3</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14866,23 +14866,23 @@
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41505376363781848</v>
+        <v>0.40658327866561811</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58439242927966384</v>
+        <v>0.55602386475152488</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61970478934388062</v>
+        <v>0.63235182586110272</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65636898498201179</v>
+        <v>0.66962896447659781</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60032157510321316</v>
+        <v>0.54837066956543501</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14890,23 +14890,23 @@
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2502047927278952</v>
+        <v>0.23534114167475287</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1933967924761654E-2</v>
+        <v>5.5760681350796724E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6568140814081463E-4</v>
+        <v>3.5161673859693715E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.0059201956960658E-5</v>
+        <v>6.189774895564313E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6645560939928683E-5</v>
+        <v>1.6322346164396085E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14931,63 +14931,63 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.529040556360012</v>
+        <v>1.5749117730508124</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4594762491382907</v>
+        <v>1.3899773801317052</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4188437606267812</v>
+        <v>1.3779155752240857</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4357641725565458</v>
+        <v>1.4220902280560073</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1486367795600976</v>
+        <v>1.136795163275973</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0765081848783828</v>
+        <v>1.013798970225273</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.89093309057953185</v>
+        <v>0.87256333613459303</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79167418447294369</v>
+        <v>0.81641400273772324</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80738282765774494</v>
+        <v>0.79930899938116751</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.73730479120212744</v>
+        <v>0.7078125995540423</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7539420028679521</v>
+        <v>0.69594646418580197</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72961055921036644</v>
+        <v>0.70793895844174171</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.6696292920198782</v>
+        <v>0.68315715650512843</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.67980387423631217</v>
+        <v>0.69979810583149782</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8058691296217384</v>
+        <v>0.88141936052377645</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14999,15 +14999,15 @@
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.124179500181226</v>
+        <v>1.0485135722844128</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0175103320335608</v>
+        <v>1.0688997427423266</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0831725115565645</v>
+        <v>1.0305913216751779</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -15015,7 +15015,7 @@
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1919627790303129</v>
+        <v>1.1465546731624914</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -15023,7 +15023,7 @@
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1793673547606227</v>
+        <v>1.2910968936326817</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -15036,11 +15036,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5423497267759557E-6</v>
+        <v>4.4969262295081963E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6134528054615828E-6</v>
+        <v>2.5350492212977355E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15064,39 +15064,39 @@
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6609065510169392E-2</v>
+        <v>9.0073428130576172E-2</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20329163933280905</v>
+        <v>0.21176212430500943</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27517507592294854</v>
+        <v>0.27801193237576244</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32566119031846791</v>
+        <v>0.33198470857707896</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34807446173288503</v>
+        <v>0.31823950787006627</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29438846471407565</v>
+        <v>0.30304694897037204</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22380578849789726</v>
+        <v>0.23294071864066859</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12014784601290016</v>
+        <v>0.12881830912723316</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6240320635669046E-2</v>
+        <v>2.7333667328821924E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15104,11 +15104,11 @@
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9723176478699916E-5</v>
+        <v>3.0029600978480329E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4843878577306387E-6</v>
+        <v>8.0803693883148939E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15137,11 +15137,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3152322404371578E-6</v>
+        <v>4.5423497267759557E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6395873335161986E-6</v>
+        <v>2.6918563896254302E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15161,27 +15161,27 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.281686909956635E-3</v>
+        <v>4.3240798496591761E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.7475156165271087E-2</v>
+        <v>9.0073428130576172E-2</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2223502305202599</v>
+        <v>0.22023260927720981</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28652250173420413</v>
+        <v>0.27517507592294854</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32566119031846791</v>
+        <v>0.31933767205985686</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31492451299641977</v>
+        <v>0.34475946685923853</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15189,27 +15189,27 @@
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23065698610497576</v>
+        <v>0.22152205596220442</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12757967153947131</v>
+        <v>0.12634103395170945</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8427014021974801E-2</v>
+        <v>2.870035069526302E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7229220191249919E-4</v>
+        <v>1.7580836929846858E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2174572476943211E-5</v>
+        <v>3.1255298977601978E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.9187620005485967E-6</v>
+        <v>8.0803693883148939E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15238,11 +15238,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.4515027322404369E-6</v>
+        <v>4.5423497267759557E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.587318277406967E-6</v>
+        <v>2.5089146932431193E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15262,11 +15262,11 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1545080908490118E-3</v>
+        <v>4.4088657290642583E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.9207337475474477E-2</v>
+        <v>9.0939518785677867E-2</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15278,39 +15278,39 @@
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33198470857707896</v>
+        <v>0.31617591293055136</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.3348144822382989</v>
+        <v>0.34807446173288503</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30304694897037204</v>
+        <v>0.29438846471407565</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23294071864066859</v>
+        <v>0.22152205596220442</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.12014784601290016</v>
+        <v>0.12262512118842388</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7060330655533704E-2</v>
+        <v>2.7880340675398362E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7756645299145325E-4</v>
+        <v>1.7932453668443796E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0029600978480329E-5</v>
+        <v>3.0642449978041152E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.1611730821980425E-6</v>
+        <v>8.3227804699643415E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26461,11 +26461,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1883695355191256E-5</v>
+        <v>1.1652943989071037E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2566060162750292E-6</v>
+        <v>6.849337112553717E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26485,39 +26485,39 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0782316273113355E-2</v>
+        <v>1.1099443222322572E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22732785417890827</v>
+        <v>0.20984109616514607</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56631438924049882</v>
+        <v>0.55013397811934173</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70491131920435146</v>
+        <v>0.72671270021067158</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79948287177884703</v>
+        <v>0.80747770049663548</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.85900953437868155</v>
+        <v>0.82532288597167447</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70781811114969995</v>
+        <v>0.71519121647417605</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60279700633245825</v>
+        <v>0.55112869150396182</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31358948067352771</v>
+        <v>0.30737978798692317</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26525,15 +26525,15 @@
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3463542629937818E-4</v>
+        <v>4.1707439897415078E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.4438097284447284E-5</v>
+        <v>7.5189997257017459E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8772314162933162E-5</v>
+        <v>1.9163404041327603E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26558,83 +26558,83 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1682471750529713</v>
+        <v>1.1001939415547399</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.98755327692775052</v>
+        <v>1.0274544194298818</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0026781720066478</v>
+        <v>1.0444564291735914</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0464699630771885</v>
+        <v>1.0565321742606231</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.92364607016172828</v>
+        <v>0.88812122130935411</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81673164100137641</v>
+        <v>0.785013907370255</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70628038423219119</v>
+        <v>0.72054867482274065</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61451318968239854</v>
+        <v>0.67212380121512338</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60438420273330917</v>
+        <v>0.61030953805422405</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55015051212938026</v>
+        <v>0.56104458167649662</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52694597830958978</v>
+        <v>0.5324927780812696</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55178165503276777</v>
+        <v>0.51428193090432717</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.49957843024895776</v>
+        <v>0.50956999885393695</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53171500275750638</v>
+        <v>0.48613943109257712</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65292290419947263</v>
+        <v>0.62183133733283102</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.68352978650965457</v>
+        <v>0.72537854894902121</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71616650131849258</v>
+        <v>0.73723022194550714</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82477952889967687</v>
+        <v>0.79305723932661232</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7770735176713337</v>
+        <v>0.75444030841877052</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.78728603852334111</v>
+        <v>0.82665034044950825</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26642,15 +26642,15 @@
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80615472782578956</v>
+        <v>0.83974450815186408</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80657775574931456</v>
+        <v>0.78188659996107024</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.92230085701649034</v>
+        <v>0.95956553810806577</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -26663,11 +26663,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.0572233606557376E-6</v>
+        <v>5.9995355191256833E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2600210295327783E-6</v>
+        <v>3.3588095455792263E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26687,39 +26687,39 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4440126280915473E-3</v>
+        <v>5.5497216111612862E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10929223758601359</v>
+        <v>0.1038276257067129</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28315719462024941</v>
+        <v>0.25618984275165418</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37425704060849585</v>
+        <v>0.37789060410954922</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37975436409495233</v>
+        <v>0.41573109332500047</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42529393613846489</v>
+        <v>0.41687227403671312</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35759560823708803</v>
+        <v>0.37234181888604007</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27843480768689738</v>
+        <v>0.28417573155673032</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15213747082181045</v>
+        <v>0.15058504765015934</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26727,15 +26727,15 @@
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1292745631838224E-4</v>
+        <v>2.0853719948707539E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6091198683368379E-5</v>
+        <v>3.8346898601078904E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.5817020206638013E-6</v>
+        <v>9.4839295510651903E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26764,11 +26764,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.7110963114754101E-6</v>
+        <v>6.0572233606557376E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1283030081375146E-6</v>
+        <v>3.2929505348815944E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26788,23 +26788,23 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3383036450218085E-3</v>
+        <v>5.4968671196264163E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10492054808257303</v>
+        <v>0.11038515996187372</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25888657793851372</v>
+        <v>0.26158331312537325</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36335635010533579</v>
+        <v>0.37425704060849585</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.39174660717163501</v>
+        <v>0.41173367896610624</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26812,7 +26812,7 @@
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37234181888604007</v>
+        <v>0.35390905557484997</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26820,23 +26820,23 @@
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15213747082181045</v>
+        <v>0.15058504765015934</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5759308024240467E-2</v>
+        <v>3.6453663519856787E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1512258473403568E-4</v>
+        <v>2.2390309839664938E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9474748559934167E-5</v>
+        <v>3.7219048642223642E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0266109307854073E-5</v>
+        <v>9.8750194294596327E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26865,11 +26865,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.0572233606557376E-6</v>
+        <v>5.5380327868852455E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1941620188351465E-6</v>
+        <v>3.1283030081375146E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26889,23 +26889,23 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3911581365566775E-3</v>
+        <v>5.074031187347461E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11257100471359399</v>
+        <v>0.11366392708945414</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26697678349909226</v>
+        <v>0.26428004831223273</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35608922310322905</v>
+        <v>0.36698991360638916</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41573109332500047</v>
+        <v>0.37975436409495233</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26913,11 +26913,11 @@
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35390905557484997</v>
+        <v>0.37602837154827812</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27269388381706444</v>
+        <v>0.29852804123131266</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26925,19 +26925,19 @@
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3676241537391509E-2</v>
+        <v>3.6106485772048627E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1731771314968909E-4</v>
+        <v>2.3048848364360966E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8346898601078904E-5</v>
+        <v>3.9098798573649079E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.7772469598610216E-6</v>
+        <v>9.28838461186797E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27216,11 +27216,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.130681693989071E-5</v>
+        <v>1.142219262295082E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.9151961232513485E-6</v>
+        <v>6.6517600804608211E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27240,43 +27240,43 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0042353391625182E-2</v>
+        <v>1.0782316273113355E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22077031992374743</v>
+        <v>0.22514200942718798</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5231666262507465</v>
+        <v>0.51777315587702744</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70491131920435146</v>
+        <v>0.71944557320856484</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80747770049663548</v>
+        <v>0.79148804306105858</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80005789966641905</v>
+        <v>0.85900953437868155</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75942984842103223</v>
+        <v>0.73731053244760414</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58557423472295944</v>
+        <v>0.5798333108531265</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32600886604673673</v>
+        <v>0.29806524895701642</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.5963772083550379E-2</v>
+        <v>7.0824260552864615E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27284,11 +27284,11 @@
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.6693797202157809E-5</v>
+        <v>7.8197597147298159E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9750038858919265E-5</v>
+        <v>1.9945583798116484E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27313,35 +27313,35 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1569049694699327</v>
+        <v>1.0775095303886628</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.98755327692775052</v>
+        <v>0.95762742005115198</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0549009934653273</v>
+        <v>1.0966792506322711</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0464699630771885</v>
+        <v>1.036407751893754</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.93252728237482185</v>
+        <v>0.87035879688316709</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80880220759359611</v>
+        <v>0.8246610744091567</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69201209364164185</v>
+        <v>0.72768282011801522</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61451318968239854</v>
+        <v>0.60811201062320686</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27349,27 +27349,27 @@
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53380940780870556</v>
+        <v>0.57193865122361309</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5324927780812696</v>
+        <v>0.5491331773963094</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51963903435124725</v>
+        <v>0.53571034469200751</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.49458264594646817</v>
+        <v>0.48459107734148904</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53171500275750638</v>
+        <v>0.5063952407214346</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64670459082614429</v>
+        <v>0.62183133733283102</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27377,11 +27377,11 @@
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71616650131849258</v>
+        <v>0.68808154048247339</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.78512666693334621</v>
+        <v>0.80891838411314465</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27389,23 +27389,23 @@
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81877748006427487</v>
+        <v>0.81090461967904137</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83845332823370533</v>
+        <v>0.90760411819112441</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81455217290730808</v>
+        <v>0.83974450815186408</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.78188659996107024</v>
+        <v>0.80657775574931456</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.93161702728938423</v>
+        <v>0.92230085701649034</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27418,7 +27418,7 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6534084699453549E-6</v>
+        <v>5.4803449453551911E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27442,7 +27442,7 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.12688567888233E-3</v>
+        <v>5.4968671196264163E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27450,39 +27450,39 @@
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27776372424653034</v>
+        <v>0.2696735186859518</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.38152416761060259</v>
+        <v>0.34518853260006899</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41173367896610624</v>
+        <v>0.38774919281274078</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.40423978088408541</v>
+        <v>0.43371559824021666</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37234181888604007</v>
+        <v>0.37602837154827812</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28417573155673032</v>
+        <v>0.27269388381706444</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16145200985171723</v>
+        <v>0.15213747082181045</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4717774780815988E-2</v>
+        <v>3.5759308024240467E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1512258473403568E-4</v>
+        <v>2.3048848364360966E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27490,7 +27490,7 @@
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.4839295510651903E-6</v>
+        <v>9.7772469598610216E-6</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27519,11 +27519,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.7110963114754101E-6</v>
+        <v>5.7687841530054644E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1283030081375146E-6</v>
+        <v>3.1941620188351465E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27543,23 +27543,23 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.074031187347461E-3</v>
+        <v>5.2325946619520688E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11147808233773386</v>
+        <v>0.11257100471359399</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25618984275165418</v>
+        <v>0.2696735186859518</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35245565960217573</v>
+        <v>0.36335635010533579</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.39574402153052929</v>
+        <v>0.40773626460721202</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27567,11 +27567,11 @@
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37234181888604007</v>
+        <v>0.35759560823708803</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28991665542656325</v>
+        <v>0.28704619349164678</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27579,19 +27579,19 @@
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4023419285199669E-2</v>
+        <v>3.5759308024240467E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3048848364360966E-4</v>
+        <v>2.0853719948707539E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8722848587363992E-5</v>
+        <v>3.8346898601078904E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0168336838255462E-5</v>
+        <v>9.5817020206638013E-6</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27620,11 +27620,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4803449453551911E-6</v>
+        <v>5.9418476775956281E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1941620188351465E-6</v>
+        <v>3.3588095455792263E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27644,39 +27644,39 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.0211766958125912E-3</v>
+        <v>5.3383036450218085E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11257100471359399</v>
+        <v>0.1038276257067129</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.27506698905967086</v>
+        <v>0.28315719462024941</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35608922310322905</v>
+        <v>0.37425704060849585</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.40773626460721202</v>
+        <v>0.38375177845384656</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4379264292910926</v>
+        <v>0.42950476718934077</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37602837154827812</v>
+        <v>0.37234181888604007</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30139850316622913</v>
+        <v>0.28417573155673032</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15058504765015934</v>
+        <v>0.1598995866800661</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27684,15 +27684,15 @@
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2390309839664938E-4</v>
+        <v>2.2170796998099597E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6467148669653467E-5</v>
+        <v>3.9098798573649079E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0266109307854073E-5</v>
+        <v>1.0168336838255462E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27890,11 +27890,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0960689890710382E-5</v>
+        <v>1.2114446721311475E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.3224650269726606E-6</v>
+        <v>6.7176190911584525E-6</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27914,55 +27914,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0676607290043617E-2</v>
+        <v>1.0782316273113355E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22732785417890827</v>
+        <v>0.22951369893062853</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52856009662446546</v>
+        <v>0.55552744849306068</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70491131920435146</v>
+        <v>0.74124695421488507</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76750355690769312</v>
+        <v>0.79148804306105858</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83374454807342624</v>
+        <v>0.82532288597167447</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70781811114969995</v>
+        <v>0.71519121647417605</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60279700633245825</v>
+        <v>0.5798333108531265</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32290401970343446</v>
+        <v>0.31358948067352771</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1518616048480935E-2</v>
+        <v>7.2212971544097254E-2</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5219645362460563E-4</v>
+        <v>4.2585491263676448E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.3686197311877109E-5</v>
+        <v>7.2182397366736759E-5</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8772314162933162E-5</v>
+        <v>1.9750038858919265E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27987,11 +27987,11 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1115361471377785</v>
+        <v>1.1455627638868942</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0474049906809475</v>
+        <v>0.97757799130221756</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27999,43 +27999,43 @@
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.97603448479314692</v>
+        <v>1.0062211183434506</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.90588364573554114</v>
+        <v>0.84371516024388638</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80087277418581571</v>
+        <v>0.77708447396247471</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71341452952746587</v>
+        <v>0.69914623893691652</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62091436874159012</v>
+        <v>0.61451318968239854</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.6221602086960536</v>
+        <v>0.58068286144964998</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52836237303514733</v>
+        <v>0.5555975469029385</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.52694597830958978</v>
+        <v>0.53803957785294954</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5410674481389276</v>
+        <v>0.51428193090432717</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.48958686164397858</v>
+        <v>0.47459950873650986</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28043,23 +28043,23 @@
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61561302395950268</v>
+        <v>0.64048627745281594</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70445416772933789</v>
+        <v>0.73235334268891561</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72318774152749743</v>
+        <v>0.73020898173650228</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82477952889967687</v>
+        <v>0.83271010129294298</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75444030841877052</v>
+        <v>0.76198471150295821</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28067,19 +28067,19 @@
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82980947948902806</v>
+        <v>0.88167257195709225</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79775728274427082</v>
+        <v>0.84814195323338282</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83126891153755889</v>
+        <v>0.80657775574931456</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.91298468674359656</v>
+        <v>0.97819787865385355</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -28092,11 +28092,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8841598360655738E-6</v>
+        <v>5.9995355191256833E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4575980616256742E-6</v>
+        <v>3.2270915241839626E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28116,7 +28116,7 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.12688567888233E-3</v>
+        <v>5.074031187347461E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28124,39 +28124,39 @@
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26158331312537325</v>
+        <v>0.25888657793851372</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35608922310322905</v>
+        <v>0.36698991360638916</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41173367896610624</v>
+        <v>0.39574402153052929</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4379264292910926</v>
+        <v>0.40845061193496135</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35022250291261198</v>
+        <v>0.37602837154827812</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28417573155673032</v>
+        <v>0.30139850316622913</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15213747082181045</v>
+        <v>0.1598995866800661</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4717774780815988E-2</v>
+        <v>3.4370597033007828E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2829335522795623E-4</v>
+        <v>2.3048848364360966E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28164,7 +28164,7 @@
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.7772469598610216E-6</v>
+        <v>1.0168336838255462E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28193,11 +28193,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8841598360655738E-6</v>
+        <v>5.8264719945355187E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2600210295327783E-6</v>
+        <v>3.3258800402304106E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28217,15 +28217,15 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4968671196264163E-3</v>
+        <v>5.4440126280915473E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11038515996187372</v>
+        <v>0.1038276257067129</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25618984275165418</v>
+        <v>0.28046045943338987</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28233,19 +28233,19 @@
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.38375177845384656</v>
+        <v>0.37975436409495233</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41687227403671312</v>
+        <v>0.40002894983320952</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37234181888604007</v>
+        <v>0.36128216089932602</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29852804123131266</v>
+        <v>0.27843480768689738</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28253,15 +28253,15 @@
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4717774780815988E-2</v>
+        <v>3.6106485772048627E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1731771314968909E-4</v>
+        <v>2.3048848364360966E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5715248697083292E-5</v>
+        <v>3.6843098655938554E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28294,11 +28294,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8841598360655738E-6</v>
+        <v>5.5957206284153006E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1612325134863303E-6</v>
+        <v>3.1941620188351465E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28318,55 +28318,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.074031187347461E-3</v>
+        <v>5.4440126280915473E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10601347045843318</v>
+        <v>0.1038276257067129</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28315719462024941</v>
+        <v>0.25888657793851372</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.37789060410954922</v>
+        <v>0.35245565960217573</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.40773626460721202</v>
+        <v>0.38375177845384656</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44213726034196849</v>
+        <v>0.42950476718934077</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35759560823708803</v>
+        <v>0.36128216089932602</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.28704619349164678</v>
+        <v>0.28417573155673032</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.15679474033676385</v>
+        <v>0.14748020130685707</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5064952528624148E-2</v>
+        <v>3.2981886041775189E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2170796998099597E-4</v>
+        <v>2.3048848364360966E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7970948614793817E-5</v>
+        <v>3.6843098655938554E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.28838461186797E-6</v>
+        <v>9.386157081466581E-6</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>

</xml_diff>